<commit_message>
Simplify group setup and fix bug in group
</commit_message>
<xml_diff>
--- a/conf/excel/catalog-newCA-config2.xlsx
+++ b/conf/excel/catalog-newCA-config2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\学习资料\综合学习资料\tencent\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\学习资料\综合学习资料\tencent\data\newCA-config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{542C1452-C4E2-4F95-A101-FD2A2403FED2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9F97CE4-828F-446E-B299-5C9BB1650067}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="1920" windowWidth="21600" windowHeight="11385" firstSheet="6" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="C_AdmArea.conf" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
     <definedName name="C_AOI" localSheetId="3">'C_AOI.conf'!$A$1:$D$1</definedName>
     <definedName name="C_BackCarto" localSheetId="4">'C_BackCarto.conf'!$A$1:$D$1</definedName>
     <definedName name="C_BackLine" localSheetId="5">'C_BackLine.conf'!$A$1:$D$99</definedName>
-    <definedName name="C_BackPolygon" localSheetId="6">'C_BackPolygon.conf'!$A$1:$Y$130</definedName>
+    <definedName name="C_BackPolygon" localSheetId="6">'C_BackPolygon.conf'!$A$1:$D$130</definedName>
     <definedName name="C_BackPolygonLine" localSheetId="7">'C_BackPolygonLine.conf'!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -123,7 +123,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1729" uniqueCount="889">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1728" uniqueCount="888">
   <si>
     <t>catalog=0804</t>
   </si>
@@ -2553,9 +2553,6 @@
   </si>
   <si>
     <t>精细化绿地</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   </t>
   </si>
   <si>
     <t>id=SHDSN0001</t>
@@ -8003,10 +8000,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27E863AC-131C-454F-92A7-2CFA7FBF776C}">
-  <dimension ref="A1:Y130"/>
+  <dimension ref="A1:D130"/>
   <sheetViews>
-    <sheetView topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="D116" sqref="A116:D117"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -8014,7 +8011,6 @@
     <col min="1" max="1" width="63.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -8545,7 +8541,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>629</v>
       </c>
@@ -8556,7 +8552,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>632</v>
       </c>
@@ -8567,7 +8563,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>635</v>
       </c>
@@ -8578,7 +8574,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>638</v>
       </c>
@@ -8589,7 +8585,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>641</v>
       </c>
@@ -8600,7 +8596,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>807</v>
       </c>
@@ -8610,11 +8606,8 @@
       <c r="D54" t="s">
         <v>809</v>
       </c>
-      <c r="Y54" t="s">
-        <v>810</v>
-      </c>
-    </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>644</v>
       </c>
@@ -8625,7 +8618,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>647</v>
       </c>
@@ -8636,7 +8629,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>650</v>
       </c>
@@ -8647,7 +8640,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>653</v>
       </c>
@@ -8658,7 +8651,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>656</v>
       </c>
@@ -8669,7 +8662,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>659</v>
       </c>
@@ -8680,7 +8673,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>661</v>
       </c>
@@ -8691,7 +8684,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>664</v>
       </c>
@@ -8702,7 +8695,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>667</v>
       </c>
@@ -8713,7 +8706,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="64" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>670</v>
       </c>
@@ -9111,200 +9104,200 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
+        <v>810</v>
+      </c>
+      <c r="B100" t="s">
         <v>811</v>
       </c>
-      <c r="B100" t="s">
+      <c r="D100" t="s">
         <v>812</v>
-      </c>
-      <c r="D100" t="s">
-        <v>813</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
+        <v>813</v>
+      </c>
+      <c r="B101" t="s">
         <v>814</v>
       </c>
-      <c r="B101" t="s">
+      <c r="D101" t="s">
         <v>815</v>
-      </c>
-      <c r="D101" t="s">
-        <v>816</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
+        <v>816</v>
+      </c>
+      <c r="B102" t="s">
         <v>817</v>
       </c>
-      <c r="B102" t="s">
+      <c r="D102" t="s">
         <v>818</v>
-      </c>
-      <c r="D102" t="s">
-        <v>819</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
+        <v>819</v>
+      </c>
+      <c r="B103" t="s">
         <v>820</v>
       </c>
-      <c r="B103" t="s">
+      <c r="D103" t="s">
         <v>821</v>
-      </c>
-      <c r="D103" t="s">
-        <v>822</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
+        <v>822</v>
+      </c>
+      <c r="B104" t="s">
         <v>823</v>
       </c>
-      <c r="B104" t="s">
+      <c r="D104" t="s">
         <v>824</v>
-      </c>
-      <c r="D104" t="s">
-        <v>825</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
+        <v>825</v>
+      </c>
+      <c r="B105" t="s">
         <v>826</v>
       </c>
-      <c r="B105" t="s">
+      <c r="D105" t="s">
         <v>827</v>
-      </c>
-      <c r="D105" t="s">
-        <v>828</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
+        <v>828</v>
+      </c>
+      <c r="B106" t="s">
         <v>829</v>
       </c>
-      <c r="B106" t="s">
+      <c r="D106" t="s">
         <v>830</v>
-      </c>
-      <c r="D106" t="s">
-        <v>831</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
+        <v>831</v>
+      </c>
+      <c r="B107" t="s">
         <v>832</v>
       </c>
-      <c r="B107" t="s">
+      <c r="D107" t="s">
         <v>833</v>
-      </c>
-      <c r="D107" t="s">
-        <v>834</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
+        <v>834</v>
+      </c>
+      <c r="B108" t="s">
         <v>835</v>
       </c>
-      <c r="B108" t="s">
+      <c r="D108" t="s">
         <v>836</v>
-      </c>
-      <c r="D108" t="s">
-        <v>837</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
+        <v>837</v>
+      </c>
+      <c r="B109" t="s">
         <v>838</v>
       </c>
-      <c r="B109" t="s">
+      <c r="D109" t="s">
         <v>839</v>
-      </c>
-      <c r="D109" t="s">
-        <v>840</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
+        <v>840</v>
+      </c>
+      <c r="B110" t="s">
         <v>841</v>
       </c>
-      <c r="B110" t="s">
+      <c r="D110" t="s">
         <v>842</v>
-      </c>
-      <c r="D110" t="s">
-        <v>843</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
+        <v>843</v>
+      </c>
+      <c r="B111" t="s">
         <v>844</v>
       </c>
-      <c r="B111" t="s">
+      <c r="D111" t="s">
         <v>845</v>
-      </c>
-      <c r="D111" t="s">
-        <v>846</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
+        <v>846</v>
+      </c>
+      <c r="B112" t="s">
         <v>847</v>
       </c>
-      <c r="B112" t="s">
+      <c r="D112" t="s">
         <v>848</v>
-      </c>
-      <c r="D112" t="s">
-        <v>849</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
+        <v>849</v>
+      </c>
+      <c r="B113" t="s">
         <v>850</v>
       </c>
-      <c r="B113" t="s">
+      <c r="D113" t="s">
         <v>851</v>
-      </c>
-      <c r="D113" t="s">
-        <v>852</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
+        <v>852</v>
+      </c>
+      <c r="B114" t="s">
         <v>853</v>
       </c>
-      <c r="B114" t="s">
+      <c r="D114" t="s">
         <v>854</v>
-      </c>
-      <c r="D114" t="s">
-        <v>855</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
+        <v>855</v>
+      </c>
+      <c r="B115" t="s">
         <v>856</v>
       </c>
-      <c r="B115" t="s">
+      <c r="D115" t="s">
         <v>857</v>
-      </c>
-      <c r="D115" t="s">
-        <v>858</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
+        <v>858</v>
+      </c>
+      <c r="B116" t="s">
         <v>859</v>
       </c>
-      <c r="B116" t="s">
+      <c r="D116" t="s">
         <v>860</v>
-      </c>
-      <c r="D116" t="s">
-        <v>861</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
+        <v>861</v>
+      </c>
+      <c r="B117" t="s">
         <v>862</v>
       </c>
-      <c r="B117" t="s">
+      <c r="D117" t="s">
         <v>863</v>
-      </c>
-      <c r="D117" t="s">
-        <v>864</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
@@ -9315,139 +9308,139 @@
         <v>615</v>
       </c>
       <c r="D118" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="B119" t="s">
         <v>808</v>
       </c>
       <c r="D119" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
+        <v>866</v>
+      </c>
+      <c r="B120" t="s">
         <v>867</v>
       </c>
-      <c r="B120" t="s">
-        <v>868</v>
-      </c>
       <c r="D120" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
+        <v>868</v>
+      </c>
+      <c r="B121" t="s">
         <v>869</v>
       </c>
-      <c r="B121" t="s">
-        <v>870</v>
-      </c>
       <c r="D121" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
+        <v>870</v>
+      </c>
+      <c r="B122" t="s">
         <v>871</v>
       </c>
-      <c r="B122" t="s">
-        <v>872</v>
-      </c>
       <c r="D122" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
+        <v>872</v>
+      </c>
+      <c r="B123" t="s">
         <v>873</v>
       </c>
-      <c r="B123" t="s">
-        <v>874</v>
-      </c>
       <c r="D123" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
+        <v>874</v>
+      </c>
+      <c r="B124" t="s">
         <v>875</v>
       </c>
-      <c r="B124" t="s">
-        <v>876</v>
-      </c>
       <c r="D124" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
+        <v>876</v>
+      </c>
+      <c r="B125" t="s">
         <v>877</v>
       </c>
-      <c r="B125" t="s">
-        <v>878</v>
-      </c>
       <c r="D125" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
+        <v>878</v>
+      </c>
+      <c r="B126" t="s">
         <v>879</v>
       </c>
-      <c r="B126" t="s">
-        <v>880</v>
-      </c>
       <c r="D126" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
+        <v>880</v>
+      </c>
+      <c r="B127" t="s">
         <v>881</v>
       </c>
-      <c r="B127" t="s">
-        <v>882</v>
-      </c>
       <c r="D127" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
+        <v>882</v>
+      </c>
+      <c r="B128" t="s">
         <v>883</v>
       </c>
-      <c r="B128" t="s">
-        <v>884</v>
-      </c>
       <c r="D128" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
+        <v>884</v>
+      </c>
+      <c r="B129" t="s">
         <v>885</v>
       </c>
-      <c r="B129" t="s">
-        <v>886</v>
-      </c>
       <c r="D129" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
+        <v>886</v>
+      </c>
+      <c r="B130" t="s">
         <v>887</v>
       </c>
-      <c r="B130" t="s">
-        <v>888</v>
-      </c>
       <c r="D130" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
   </sheetData>
@@ -9460,7 +9453,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07FB1634-467C-436D-BAF8-F9871795E23F}">
   <dimension ref="B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update with more accurate debug info
</commit_message>
<xml_diff>
--- a/conf/excel/catalog-newCA-config2.xlsx
+++ b/conf/excel/catalog-newCA-config2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\学习资料\综合学习资料\tencent\data\newCA-config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9F97CE4-828F-446E-B299-5C9BB1650067}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{849DBCF5-78D7-480E-80AD-810F24FB9A74}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -123,7 +123,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1728" uniqueCount="888">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1728" uniqueCount="891">
   <si>
     <t>catalog=0804</t>
   </si>
@@ -2787,6 +2787,18 @@
   </si>
   <si>
     <t>catalog=090215</t>
+  </si>
+  <si>
+    <t>kind=013a0 || kind=01320</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kind=1001 || kind=1002</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kind=3001 || kind=3002</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -8002,8 +8014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27E863AC-131C-454F-92A7-2CFA7FBF776C}">
   <dimension ref="A1:D130"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
+      <selection activeCell="A123" sqref="A123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -8400,7 +8412,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>611</v>
+        <v>888</v>
       </c>
       <c r="B36" t="s">
         <v>612</v>
@@ -8697,7 +8709,7 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>667</v>
+        <v>889</v>
       </c>
       <c r="B63" t="s">
         <v>668</v>
@@ -8719,7 +8731,7 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>673</v>
+        <v>890</v>
       </c>
       <c r="B65" t="s">
         <v>674</v>
@@ -9446,6 +9458,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>